<commit_message>
Corrected the line number
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -15,84 +15,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Line_1</t>
   </si>
   <si>
+    <t>Line_10</t>
+  </si>
+  <si>
+    <t>Line_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Line_2</t>
+  </si>
+  <si>
+    <t>Line_11</t>
+  </si>
+  <si>
+    <t>Line_20</t>
+  </si>
+  <si>
+    <t>Line_3</t>
+  </si>
+  <si>
+    <t>Line_12</t>
+  </si>
+  <si>
+    <t>Line_21</t>
+  </si>
+  <si>
+    <t>Line_4</t>
+  </si>
+  <si>
+    <t>Line_13</t>
+  </si>
+  <si>
+    <t>Line_22</t>
+  </si>
+  <si>
+    <t>Line_5</t>
+  </si>
+  <si>
+    <t>Line_14</t>
+  </si>
+  <si>
+    <t>Line_23</t>
+  </si>
+  <si>
+    <t>Line_6</t>
+  </si>
+  <si>
+    <t>Line_15</t>
+  </si>
+  <si>
+    <t>Line_24</t>
+  </si>
+  <si>
+    <t>Line_7</t>
+  </si>
+  <si>
+    <t>Line_16</t>
+  </si>
+  <si>
+    <t>Line_25</t>
+  </si>
+  <si>
+    <t>Line_8</t>
+  </si>
+  <si>
+    <t>Line_17</t>
+  </si>
+  <si>
+    <t>Line_26</t>
+  </si>
+  <si>
     <t>Line_9</t>
   </si>
   <si>
     <t>Line_18</t>
   </si>
   <si>
-    <t xml:space="preserve">	</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Line_2</t>
-  </si>
-  <si>
-    <t>Line_10</t>
-  </si>
-  <si>
-    <t>Line_19</t>
-  </si>
-  <si>
-    <t>Line_3</t>
-  </si>
-  <si>
-    <t>Line_11</t>
-  </si>
-  <si>
-    <t>Line_20</t>
-  </si>
-  <si>
-    <t>Line_4</t>
-  </si>
-  <si>
-    <t>Line_12</t>
-  </si>
-  <si>
-    <t>Line_21</t>
-  </si>
-  <si>
-    <t>Line_5</t>
-  </si>
-  <si>
-    <t>Line_13</t>
-  </si>
-  <si>
-    <t>Line_22</t>
-  </si>
-  <si>
-    <t>Line_6</t>
-  </si>
-  <si>
-    <t>Line_14</t>
-  </si>
-  <si>
-    <t>Line_23</t>
-  </si>
-  <si>
-    <t>Line_7</t>
-  </si>
-  <si>
-    <t>Line_15</t>
-  </si>
-  <si>
-    <t>Line_24</t>
-  </si>
-  <si>
-    <t>Line_8</t>
-  </si>
-  <si>
-    <t>Line_16</t>
-  </si>
-  <si>
-    <t>Line_25</t>
+    <t>Line_27</t>
   </si>
 </sst>
 </file>
@@ -377,11 +386,11 @@
     <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="14" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="2" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="8" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="13" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="12" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="14" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -760,8 +769,8 @@
       <c r="T3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="U3" s="5" t="s">
-        <v>4</v>
+      <c r="U3" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="V3" s="3" t="s">
         <v>3</v>
@@ -854,8 +863,8 @@
       <c r="T5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="U5" s="12" t="s">
-        <v>3</v>
+      <c r="U5" s="14" t="s">
+        <v>4</v>
       </c>
       <c r="V5" s="12" t="s">
         <v>3</v>
@@ -877,7 +886,7 @@
       </c>
     </row>
     <row r="8" spans="1:25">
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="15" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -889,7 +898,7 @@
       <c r="J8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="16" t="s">
         <v>4</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -913,8 +922,8 @@
       <c r="T8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="U8" s="3" t="s">
-        <v>3</v>
+      <c r="U8" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="V8" s="3" t="s">
         <v>3</v>
@@ -924,7 +933,7 @@
       </c>
     </row>
     <row r="9" spans="1:25">
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -936,7 +945,7 @@
       <c r="J9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="K9" s="18" t="s">
         <v>3</v>
       </c>
       <c r="M9" s="6" t="s">
@@ -954,20 +963,20 @@
       <c r="Q9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="S9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="T9" s="7" t="s">
-        <v>4</v>
+      <c r="S9" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="U9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="V9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="W9" s="8" t="s">
-        <v>4</v>
+      <c r="V9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="W9" s="18" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -989,32 +998,32 @@
       <c r="M10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="N10" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="O10" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="P10" s="18" t="s">
+      <c r="N10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10" s="14" t="s">
         <v>4</v>
       </c>
       <c r="Q10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="S10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="T10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="U10" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="V10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="W10" s="13" t="s">
-        <v>3</v>
+      <c r="S10" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="T10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="U10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="V10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="W10" s="20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:25"/>
@@ -1060,24 +1069,24 @@
       <c r="Q13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W13" s="4" t="s">
-        <v>3</v>
+      <c r="S13" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="W13" s="16" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:25">
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H14" s="9" t="s">
@@ -1089,10 +1098,10 @@
       <c r="J14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="M14" s="16" t="s">
+      <c r="K14" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" s="17" t="s">
         <v>3</v>
       </c>
       <c r="N14" s="9" t="s">
@@ -1104,10 +1113,10 @@
       <c r="P14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="Q14" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="S14" s="16" t="s">
+      <c r="Q14" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="S14" s="17" t="s">
         <v>3</v>
       </c>
       <c r="T14" s="9" t="s">
@@ -1119,7 +1128,7 @@
       <c r="V14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="W14" s="17" t="s">
+      <c r="W14" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1127,13 +1136,13 @@
       <c r="G15" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="J15" s="18" t="s">
+      <c r="H15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="14" t="s">
         <v>4</v>
       </c>
       <c r="K15" s="20" t="s">
@@ -1142,32 +1151,32 @@
       <c r="M15" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="N15" s="18" t="s">
+      <c r="N15" s="14" t="s">
         <v>4</v>
       </c>
       <c r="O15" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="P15" s="18" t="s">
+      <c r="P15" s="14" t="s">
         <v>4</v>
       </c>
       <c r="Q15" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="S15" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="T15" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="U15" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="V15" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="W15" s="20" t="s">
-        <v>4</v>
+      <c r="S15" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="T15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="U15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="V15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="W15" s="13" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:25"/>
@@ -1183,7 +1192,7 @@
       </c>
     </row>
     <row r="18" spans="1:25">
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="15" t="s">
         <v>4</v>
       </c>
       <c r="H18" s="3" t="s">
@@ -1195,10 +1204,10 @@
       <c r="J18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K18" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="M18" s="14" t="s">
+      <c r="K18" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" s="15" t="s">
         <v>4</v>
       </c>
       <c r="N18" s="5" t="s">
@@ -1210,10 +1219,10 @@
       <c r="P18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="Q18" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="S18" s="14" t="s">
+      <c r="Q18" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="S18" s="15" t="s">
         <v>4</v>
       </c>
       <c r="T18" s="5" t="s">
@@ -1222,15 +1231,15 @@
       <c r="U18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="V18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="W18" s="15" t="s">
-        <v>4</v>
+      <c r="V18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W18" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:25">
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H19" s="7" t="s">
@@ -1242,10 +1251,10 @@
       <c r="J19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K19" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="M19" s="16" t="s">
+      <c r="K19" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M19" s="17" t="s">
         <v>3</v>
       </c>
       <c r="N19" s="9" t="s">
@@ -1257,22 +1266,22 @@
       <c r="P19" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="Q19" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="S19" s="16" t="s">
+      <c r="Q19" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="S19" s="17" t="s">
         <v>3</v>
       </c>
       <c r="T19" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="U19" s="9" t="s">
-        <v>3</v>
+      <c r="U19" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="V19" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="W19" s="17" t="s">
+      <c r="W19" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1283,7 +1292,7 @@
       <c r="H20" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="18" t="s">
+      <c r="I20" s="14" t="s">
         <v>4</v>
       </c>
       <c r="J20" s="12" t="s">
@@ -1313,14 +1322,14 @@
       <c r="T20" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="U20" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="V20" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="W20" s="13" t="s">
-        <v>3</v>
+      <c r="U20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="V20" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="W20" s="20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:25"/>
@@ -1366,24 +1375,24 @@
       <c r="Q23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S23" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="T23" s="5" t="s">
-        <v>4</v>
+      <c r="S23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="U23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="V23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W23" s="4" t="s">
-        <v>3</v>
+      <c r="V23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="W23" s="16" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:25">
-      <c r="G24" s="16" t="s">
+      <c r="G24" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H24" s="7" t="s">
@@ -1395,10 +1404,10 @@
       <c r="J24" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K24" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="M24" s="16" t="s">
+      <c r="K24" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M24" s="17" t="s">
         <v>3</v>
       </c>
       <c r="N24" s="7" t="s">
@@ -1410,10 +1419,10 @@
       <c r="P24" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Q24" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="S24" s="16" t="s">
+      <c r="Q24" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="S24" s="17" t="s">
         <v>3</v>
       </c>
       <c r="T24" s="9" t="s">
@@ -1425,7 +1434,7 @@
       <c r="V24" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="W24" s="17" t="s">
+      <c r="W24" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1460,20 +1469,20 @@
       <c r="Q25" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="S25" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="T25" s="12" t="s">
-        <v>3</v>
+      <c r="S25" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="T25" s="14" t="s">
+        <v>4</v>
       </c>
       <c r="U25" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="V25" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="W25" s="20" t="s">
-        <v>4</v>
+      <c r="V25" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="W25" s="13" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:25"/>
@@ -1504,7 +1513,7 @@
       <c r="K28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M28" s="14" t="s">
+      <c r="M28" s="15" t="s">
         <v>4</v>
       </c>
       <c r="N28" s="3" t="s">
@@ -1516,14 +1525,14 @@
       <c r="P28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q28" s="15" t="s">
+      <c r="Q28" s="16" t="s">
         <v>4</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="T28" s="3" t="s">
-        <v>3</v>
+      <c r="T28" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="U28" s="3" t="s">
         <v>3</v>
@@ -1531,8 +1540,8 @@
       <c r="V28" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="W28" s="15" t="s">
-        <v>4</v>
+      <c r="W28" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:25">
@@ -1551,7 +1560,7 @@
       <c r="K29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M29" s="16" t="s">
+      <c r="M29" s="17" t="s">
         <v>3</v>
       </c>
       <c r="N29" s="7" t="s">
@@ -1563,23 +1572,23 @@
       <c r="P29" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Q29" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="S29" s="16" t="s">
-        <v>3</v>
+      <c r="Q29" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="S29" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="T29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="U29" s="7" t="s">
-        <v>4</v>
+      <c r="U29" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="V29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="W29" s="17" t="s">
-        <v>3</v>
+      <c r="W29" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:25">
@@ -1613,14 +1622,14 @@
       <c r="Q30" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="S30" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="T30" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="U30" s="12" t="s">
-        <v>3</v>
+      <c r="S30" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="T30" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="U30" s="14" t="s">
+        <v>4</v>
       </c>
       <c r="V30" s="12" t="s">
         <v>3</v>
@@ -1657,7 +1666,7 @@
       <c r="K33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M33" s="14" t="s">
+      <c r="M33" s="15" t="s">
         <v>4</v>
       </c>
       <c r="N33" s="3" t="s">
@@ -1669,20 +1678,20 @@
       <c r="P33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q33" s="15" t="s">
+      <c r="Q33" s="16" t="s">
         <v>4</v>
       </c>
       <c r="S33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="T33" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="U33" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="V33" s="5" t="s">
-        <v>4</v>
+      <c r="T33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="V33" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="W33" s="4" t="s">
         <v>3</v>
@@ -1704,7 +1713,7 @@
       <c r="K34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M34" s="16" t="s">
+      <c r="M34" s="17" t="s">
         <v>3</v>
       </c>
       <c r="N34" s="9" t="s">
@@ -1716,7 +1725,7 @@
       <c r="P34" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="Q34" s="17" t="s">
+      <c r="Q34" s="18" t="s">
         <v>3</v>
       </c>
       <c r="S34" s="6" t="s">
@@ -1739,13 +1748,13 @@
       <c r="G35" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H35" s="18" t="s">
+      <c r="H35" s="14" t="s">
         <v>4</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J35" s="18" t="s">
+      <c r="J35" s="14" t="s">
         <v>4</v>
       </c>
       <c r="K35" s="13" t="s">
@@ -1754,13 +1763,13 @@
       <c r="M35" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="N35" s="18" t="s">
+      <c r="N35" s="14" t="s">
         <v>4</v>
       </c>
       <c r="O35" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="P35" s="18" t="s">
+      <c r="P35" s="14" t="s">
         <v>4</v>
       </c>
       <c r="Q35" s="13" t="s">
@@ -1769,14 +1778,14 @@
       <c r="S35" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="T35" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="U35" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="V35" s="12" t="s">
-        <v>3</v>
+      <c r="T35" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="U35" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="V35" s="14" t="s">
+        <v>4</v>
       </c>
       <c r="W35" s="13" t="s">
         <v>3</v>
@@ -1795,7 +1804,7 @@
       </c>
     </row>
     <row r="38" spans="1:25">
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="15" t="s">
         <v>4</v>
       </c>
       <c r="H38" s="3" t="s">
@@ -1807,7 +1816,7 @@
       <c r="J38" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K38" s="15" t="s">
+      <c r="K38" s="16" t="s">
         <v>4</v>
       </c>
       <c r="M38" s="2" t="s">
@@ -1842,7 +1851,7 @@
       </c>
     </row>
     <row r="39" spans="1:25">
-      <c r="G39" s="16" t="s">
+      <c r="G39" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H39" s="7" t="s">
@@ -1854,10 +1863,10 @@
       <c r="J39" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K39" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="M39" s="16" t="s">
+      <c r="K39" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M39" s="17" t="s">
         <v>3</v>
       </c>
       <c r="N39" s="9" t="s">
@@ -1869,7 +1878,7 @@
       <c r="P39" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="Q39" s="17" t="s">
+      <c r="Q39" s="18" t="s">
         <v>3</v>
       </c>
       <c r="S39" s="6" t="s">
@@ -1910,7 +1919,7 @@
       <c r="N40" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O40" s="18" t="s">
+      <c r="O40" s="14" t="s">
         <v>4</v>
       </c>
       <c r="P40" s="12" t="s">
@@ -1922,13 +1931,13 @@
       <c r="S40" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="T40" s="18" t="s">
+      <c r="T40" s="14" t="s">
         <v>4</v>
       </c>
       <c r="U40" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="V40" s="18" t="s">
+      <c r="V40" s="14" t="s">
         <v>4</v>
       </c>
       <c r="W40" s="13" t="s">
@@ -1938,7 +1947,13 @@
     <row r="41" spans="1:25"/>
     <row r="42" spans="1:25">
       <c r="G42" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S42" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:25">
@@ -1957,9 +1972,39 @@
       <c r="K43" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="M43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U43" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="V43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W43" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="44" spans="1:25">
-      <c r="G44" s="16" t="s">
+      <c r="G44" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H44" s="7" t="s">
@@ -1971,8 +2016,38 @@
       <c r="J44" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K44" s="17" t="s">
-        <v>3</v>
+      <c r="K44" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N44" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O44" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P44" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q44" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="S44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="T44" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="U44" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="V44" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="W44" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:25">
@@ -1982,7 +2057,7 @@
       <c r="H45" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I45" s="18" t="s">
+      <c r="I45" s="14" t="s">
         <v>4</v>
       </c>
       <c r="J45" s="12" t="s">
@@ -1990,6 +2065,36 @@
       </c>
       <c r="K45" s="20" t="s">
         <v>4</v>
+      </c>
+      <c r="M45" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O45" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="P45" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q45" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="S45" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="T45" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="U45" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="V45" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="W45" s="13" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>